<commit_message>
ajustes segun nuevas directrices
Se ajusta CS_08_02_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion04/Escaleta_CS_09_04_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion04/Escaleta_CS_09_04_CO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="151">
   <si>
     <t>Asignatura</t>
   </si>
@@ -431,6 +431,48 @@
   </si>
   <si>
     <t>Incluye audio que debe solicitarse a laFontoeca Nacional tduplat@rtvc.gov.co</t>
+  </si>
+  <si>
+    <t>Practica: Los gobiernos militares</t>
+  </si>
+  <si>
+    <t>Actividad para revisar hechos relacionados con los gobiernos militares</t>
+  </si>
+  <si>
+    <t>Competencias</t>
+  </si>
+  <si>
+    <t>Competencias: Colombia en la primera mitad del siglo XX</t>
+  </si>
+  <si>
+    <t>Actividad que sintetiza los principales aspectos de la vida política colombiana a principios de siglo XX</t>
+  </si>
+  <si>
+    <t>Competencias: La Hegemonía conservadora y la República liberal</t>
+  </si>
+  <si>
+    <t>Actividad que sintetiza hechos relacionados con la Hegemonía conservadora y la República liberal</t>
+  </si>
+  <si>
+    <t>Competencias: Colombia a principios del siglo XX</t>
+  </si>
+  <si>
+    <t>Actividad que sintetiza la vida política de Colombia a principios de siglo XX</t>
+  </si>
+  <si>
+    <t>Mapa conceptual</t>
+  </si>
+  <si>
+    <t>Evaluación: Colombia en la primera mitad del siglo XX</t>
+  </si>
+  <si>
+    <t>Fin de tema</t>
+  </si>
+  <si>
+    <t>Evalúa tus conocimientos sobre la vida política de Colombia primera mitad del siglo XX</t>
+  </si>
+  <si>
+    <t>Mapa que sintetiza la vida política de Colombia a principios de siglo XX</t>
   </si>
 </sst>
 </file>
@@ -523,7 +565,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -650,19 +692,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -759,12 +788,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -780,37 +809,35 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -824,12 +851,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1112,7 +1139,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1122,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1223,33 +1250,33 @@
       <c r="D2" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="36" t="s">
+      <c r="F2" s="29"/>
+      <c r="G2" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="H2" s="37">
+      <c r="H2" s="35">
         <v>1</v>
       </c>
-      <c r="I2" s="37" t="s">
+      <c r="I2" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="J2" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="K2" s="44" t="s">
+      <c r="K2" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="L2" s="45" t="s">
+      <c r="L2" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="45" t="s">
+      <c r="M2" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="46"/>
-      <c r="O2" s="47" t="s">
+      <c r="N2" s="44"/>
+      <c r="O2" s="45" t="s">
         <v>19</v>
       </c>
       <c r="P2" s="3"/>
@@ -1259,39 +1286,47 @@
       <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="32" t="s">
+      <c r="A3" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="33"/>
-      <c r="G3" s="39" t="s">
+      <c r="F3" s="31"/>
+      <c r="G3" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="40">
+      <c r="H3" s="38">
         <v>2</v>
       </c>
-      <c r="I3" s="40" t="s">
+      <c r="I3" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="K3" s="48" t="s">
+      <c r="K3" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="L3" s="49" t="s">
+      <c r="L3" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="49" t="s">
+      <c r="M3" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="50" t="s">
+      <c r="N3" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="O3" s="47" t="s">
+      <c r="O3" s="45" t="s">
         <v>19</v>
       </c>
       <c r="P3" s="1"/>
@@ -1301,35 +1336,43 @@
       <c r="T3" s="2"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="39" t="s">
+      <c r="A4" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="30"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="H4" s="40">
+      <c r="H4" s="38">
         <v>3</v>
       </c>
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="41" t="s">
+      <c r="J4" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="K4" s="48" t="s">
+      <c r="K4" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="L4" s="49" t="s">
+      <c r="L4" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="49" t="s">
+      <c r="M4" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="N4" s="50"/>
-      <c r="O4" s="47" t="s">
+      <c r="N4" s="48"/>
+      <c r="O4" s="45" t="s">
         <v>19</v>
       </c>
       <c r="P4" s="1"/>
@@ -1339,37 +1382,45 @@
       <c r="T4" s="2"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="32" t="s">
+      <c r="A5" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="F5" s="33"/>
-      <c r="G5" s="39" t="s">
+      <c r="F5" s="31"/>
+      <c r="G5" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="H5" s="40">
+      <c r="H5" s="38">
         <v>4</v>
       </c>
-      <c r="I5" s="40" t="s">
+      <c r="I5" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="41" t="s">
+      <c r="J5" s="39" t="s">
         <v>101</v>
       </c>
-      <c r="K5" s="48" t="s">
+      <c r="K5" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="L5" s="49" t="s">
+      <c r="L5" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="49" t="s">
+      <c r="M5" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="N5" s="51"/>
-      <c r="O5" s="47" t="s">
+      <c r="N5" s="49"/>
+      <c r="O5" s="45" t="s">
         <v>19</v>
       </c>
       <c r="P5" s="1"/>
@@ -1379,23 +1430,31 @@
       <c r="T5" s="2"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="32" t="s">
+      <c r="A6" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="48"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="50"/>
-      <c r="O6" s="47"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="45"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="13"/>
       <c r="R6" s="13"/>
@@ -1403,23 +1462,31 @@
       <c r="T6" s="2"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="32" t="s">
+      <c r="A7" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="49"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="47"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="46"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="45"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="13"/>
       <c r="R7" s="13"/>
@@ -1427,39 +1494,47 @@
       <c r="T7" s="2"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="24"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="30" t="s">
+      <c r="A8" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="39" t="s">
+      <c r="F8" s="29"/>
+      <c r="G8" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="H8" s="40">
+      <c r="H8" s="38">
         <v>5</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="41" t="s">
+      <c r="J8" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="K8" s="48" t="s">
+      <c r="K8" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="L8" s="49" t="s">
+      <c r="L8" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="M8" s="49" t="s">
+      <c r="M8" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="N8" s="50" t="s">
+      <c r="N8" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="O8" s="47" t="s">
+      <c r="O8" s="45" t="s">
         <v>19</v>
       </c>
       <c r="P8" s="3"/>
@@ -1469,23 +1544,31 @@
       <c r="T8" s="4"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="32" t="s">
+      <c r="A9" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="49"/>
-      <c r="M9" s="49"/>
-      <c r="N9" s="46"/>
-      <c r="O9" s="47"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="45"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="13"/>
       <c r="R9" s="13"/>
@@ -1493,37 +1576,45 @@
       <c r="T9" s="2"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="32" t="s">
+      <c r="A10" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="33"/>
-      <c r="G10" s="39" t="s">
+      <c r="F10" s="31"/>
+      <c r="G10" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="H10" s="40">
+      <c r="H10" s="38">
         <v>6</v>
       </c>
-      <c r="I10" s="40" t="s">
+      <c r="I10" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="42" t="s">
+      <c r="J10" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="K10" s="48" t="s">
+      <c r="K10" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="L10" s="49" t="s">
+      <c r="L10" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="M10" s="49" t="s">
+      <c r="M10" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="N10" s="50"/>
-      <c r="O10" s="47" t="s">
+      <c r="N10" s="48"/>
+      <c r="O10" s="45" t="s">
         <v>19</v>
       </c>
       <c r="P10" s="1"/>
@@ -1533,25 +1624,31 @@
       <c r="T10" s="2"/>
     </row>
     <row r="11" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
+      <c r="A11" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>88</v>
+      </c>
       <c r="D11" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="33"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="49"/>
-      <c r="M11" s="49"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="47"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="45"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
@@ -1559,39 +1656,47 @@
       <c r="T11" s="2"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="32" t="s">
+      <c r="A12" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="F12" s="33"/>
-      <c r="G12" s="39" t="s">
+      <c r="F12" s="31"/>
+      <c r="G12" s="37" t="s">
         <v>114</v>
       </c>
-      <c r="H12" s="40">
+      <c r="H12" s="38">
         <v>7</v>
       </c>
-      <c r="I12" s="40" t="s">
+      <c r="I12" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="41" t="s">
+      <c r="J12" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="K12" s="48" t="s">
+      <c r="K12" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="L12" s="49" t="s">
+      <c r="L12" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="M12" s="49" t="s">
+      <c r="M12" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="N12" s="50" t="s">
+      <c r="N12" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="O12" s="47" t="s">
+      <c r="O12" s="45" t="s">
         <v>116</v>
       </c>
       <c r="P12" s="1"/>
@@ -1601,37 +1706,45 @@
       <c r="T12" s="2"/>
     </row>
     <row r="13" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="32" t="s">
+      <c r="A13" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="39" t="s">
+      <c r="F13" s="31"/>
+      <c r="G13" s="37" t="s">
         <v>118</v>
       </c>
-      <c r="H13" s="40">
+      <c r="H13" s="38">
         <v>8</v>
       </c>
-      <c r="I13" s="40" t="s">
+      <c r="I13" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="41" t="s">
+      <c r="J13" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="K13" s="48" t="s">
+      <c r="K13" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="L13" s="49" t="s">
+      <c r="L13" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="M13" s="49" t="s">
+      <c r="M13" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="N13" s="50"/>
-      <c r="O13" s="47" t="s">
+      <c r="N13" s="48"/>
+      <c r="O13" s="45" t="s">
         <v>116</v>
       </c>
       <c r="P13" s="1"/>
@@ -1641,23 +1754,31 @@
       <c r="T13" s="2"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="32" t="s">
+      <c r="A14" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E14" s="30" t="s">
         <v>120</v>
       </c>
-      <c r="F14" s="33"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="49"/>
-      <c r="M14" s="49"/>
-      <c r="N14" s="50"/>
-      <c r="O14" s="47"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="45"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="13"/>
       <c r="R14" s="13"/>
@@ -1665,23 +1786,31 @@
       <c r="T14" s="2"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="32" t="s">
+      <c r="A15" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="49"/>
-      <c r="M15" s="49"/>
-      <c r="N15" s="50"/>
-      <c r="O15" s="47"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="47"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="45"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="13"/>
       <c r="R15" s="13"/>
@@ -1689,35 +1818,43 @@
       <c r="T15" s="2"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="32" t="s">
+      <c r="A16" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="39" t="s">
+      <c r="F16" s="31"/>
+      <c r="G16" s="37" t="s">
         <v>122</v>
       </c>
-      <c r="H16" s="40">
+      <c r="H16" s="38">
         <v>9</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="41" t="s">
+      <c r="I16" s="38"/>
+      <c r="J16" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="K16" s="48" t="s">
+      <c r="K16" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="L16" s="49" t="s">
+      <c r="L16" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="M16" s="49" t="s">
+      <c r="M16" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="N16" s="50"/>
-      <c r="O16" s="47" t="s">
+      <c r="N16" s="48"/>
+      <c r="O16" s="45" t="s">
         <v>116</v>
       </c>
       <c r="P16" s="1"/>
@@ -1727,25 +1864,31 @@
       <c r="T16" s="2"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
+      <c r="A17" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>88</v>
+      </c>
       <c r="D17" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="F17" s="33"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="48"/>
-      <c r="L17" s="49"/>
-      <c r="M17" s="49"/>
-      <c r="N17" s="50"/>
-      <c r="O17" s="47"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="45"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="13"/>
       <c r="R17" s="13"/>
@@ -1753,39 +1896,47 @@
       <c r="T17" s="2"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="32" t="s">
+      <c r="A18" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="G18" s="39" t="s">
+      <c r="G18" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="H18" s="40">
+      <c r="H18" s="38">
         <v>10</v>
       </c>
-      <c r="I18" s="40"/>
-      <c r="J18" s="41" t="s">
+      <c r="I18" s="38"/>
+      <c r="J18" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="K18" s="48" t="s">
+      <c r="K18" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="L18" s="49" t="s">
+      <c r="L18" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="M18" s="49" t="s">
+      <c r="M18" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="N18" s="50" t="s">
+      <c r="N18" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="O18" s="47"/>
+      <c r="O18" s="45"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="13"/>
       <c r="R18" s="13"/>
@@ -1793,23 +1944,31 @@
       <c r="T18" s="2"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="23"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="32" t="s">
+      <c r="A19" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="E19" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="F19" s="33"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="48"/>
-      <c r="L19" s="49"/>
-      <c r="M19" s="49"/>
-      <c r="N19" s="50"/>
-      <c r="O19" s="47"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="48"/>
+      <c r="O19" s="45"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="13"/>
       <c r="R19" s="13"/>
@@ -1817,37 +1976,45 @@
       <c r="T19" s="2"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="32" t="s">
+      <c r="A20" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="F20" s="33"/>
-      <c r="G20" s="39" t="s">
+      <c r="F20" s="31"/>
+      <c r="G20" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="H20" s="40">
+      <c r="H20" s="38">
         <v>11</v>
       </c>
-      <c r="I20" s="40" t="s">
+      <c r="I20" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="41" t="s">
+      <c r="J20" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="K20" s="48" t="s">
+      <c r="K20" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="L20" s="49" t="s">
+      <c r="L20" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="M20" s="49" t="s">
+      <c r="M20" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="N20" s="50"/>
-      <c r="O20" s="47" t="s">
+      <c r="N20" s="48"/>
+      <c r="O20" s="45" t="s">
         <v>19</v>
       </c>
       <c r="P20" s="1"/>
@@ -1857,39 +2024,45 @@
       <c r="T20" s="2"/>
     </row>
     <row r="21" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="25"/>
+      <c r="A21" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>88</v>
+      </c>
       <c r="D21" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="E21" s="32"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="39" t="s">
+      <c r="E21" s="30"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="37" t="s">
         <v>134</v>
       </c>
-      <c r="H21" s="40">
+      <c r="H21" s="38">
         <v>12</v>
       </c>
-      <c r="I21" s="40" t="s">
+      <c r="I21" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="J21" s="41" t="s">
+      <c r="J21" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="K21" s="48" t="s">
+      <c r="K21" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="L21" s="49" t="s">
+      <c r="L21" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="M21" s="49" t="s">
+      <c r="M21" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="N21" s="50" t="s">
+      <c r="N21" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="O21" s="47" t="s">
+      <c r="O21" s="45" t="s">
         <v>19</v>
       </c>
       <c r="P21" s="1"/>
@@ -1899,21 +2072,47 @@
       <c r="T21" s="2"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="50"/>
-      <c r="O22" s="47"/>
+      <c r="A22" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>133</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="F22" s="31"/>
+      <c r="G22" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22" s="38">
+        <v>13</v>
+      </c>
+      <c r="I22" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="K22" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="L22" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="M22" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="N22" s="48"/>
+      <c r="O22" s="45" t="s">
+        <v>19</v>
+      </c>
       <c r="P22" s="1"/>
       <c r="Q22" s="13"/>
       <c r="R22" s="13"/>
@@ -1921,21 +2120,45 @@
       <c r="T22" s="2"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="48"/>
-      <c r="L23" s="49"/>
-      <c r="M23" s="49"/>
-      <c r="N23" s="50"/>
-      <c r="O23" s="47"/>
+      <c r="A23" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="E23" s="30"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="H23" s="38">
+        <v>14</v>
+      </c>
+      <c r="I23" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="K23" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="L23" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="M23" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="N23" s="48"/>
+      <c r="O23" s="45" t="s">
+        <v>19</v>
+      </c>
       <c r="P23" s="1"/>
       <c r="Q23" s="13"/>
       <c r="R23" s="13"/>
@@ -1943,21 +2166,45 @@
       <c r="T23" s="2"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="48"/>
-      <c r="L24" s="49"/>
-      <c r="M24" s="49"/>
-      <c r="N24" s="50"/>
-      <c r="O24" s="47"/>
+      <c r="A24" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="E24" s="30"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="H24" s="38">
+        <v>15</v>
+      </c>
+      <c r="I24" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="K24" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="L24" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="M24" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="N24" s="48"/>
+      <c r="O24" s="45" t="s">
+        <v>19</v>
+      </c>
       <c r="P24" s="1"/>
       <c r="Q24" s="13"/>
       <c r="R24" s="13"/>
@@ -1965,21 +2212,45 @@
       <c r="T24" s="2"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="33"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="48"/>
-      <c r="L25" s="49"/>
-      <c r="M25" s="49"/>
-      <c r="N25" s="50"/>
-      <c r="O25" s="47"/>
+      <c r="A25" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="E25" s="30"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="H25" s="38">
+        <v>16</v>
+      </c>
+      <c r="I25" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="K25" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="L25" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="M25" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="N25" s="48"/>
+      <c r="O25" s="45" t="s">
+        <v>19</v>
+      </c>
       <c r="P25" s="1"/>
       <c r="Q25" s="13"/>
       <c r="R25" s="13"/>
@@ -1987,21 +2258,39 @@
       <c r="T25" s="2"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="33"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="48"/>
-      <c r="L26" s="49"/>
-      <c r="M26" s="49"/>
-      <c r="N26" s="50"/>
-      <c r="O26" s="47"/>
+      <c r="A26" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" s="30"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="H26" s="38">
+        <v>17</v>
+      </c>
+      <c r="I26" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="K26" s="46"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="48"/>
+      <c r="O26" s="45" t="s">
+        <v>19</v>
+      </c>
       <c r="P26" s="1"/>
       <c r="Q26" s="13"/>
       <c r="R26" s="13"/>
@@ -2013,17 +2302,33 @@
       <c r="B27" s="24"/>
       <c r="C27" s="25"/>
       <c r="D27" s="26"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="48"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="50"/>
-      <c r="O27" s="47"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="H27" s="38">
+        <v>18</v>
+      </c>
+      <c r="I27" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="J27" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="K27" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="L27" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="M27" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="N27" s="48"/>
+      <c r="O27" s="45" t="s">
+        <v>19</v>
+      </c>
       <c r="P27" s="1"/>
       <c r="Q27" s="13"/>
       <c r="R27" s="13"/>
@@ -2035,17 +2340,17 @@
       <c r="B28" s="24"/>
       <c r="C28" s="25"/>
       <c r="D28" s="26"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="48"/>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="50"/>
-      <c r="O28" s="47"/>
+      <c r="E28" s="30"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="47"/>
+      <c r="M28" s="47"/>
+      <c r="N28" s="48"/>
+      <c r="O28" s="45"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="13"/>
       <c r="R28" s="13"/>
@@ -2057,17 +2362,17 @@
       <c r="B29" s="24"/>
       <c r="C29" s="25"/>
       <c r="D29" s="26"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="33"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="49"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="50"/>
-      <c r="O29" s="47"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="47"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="48"/>
+      <c r="O29" s="45"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="13"/>
       <c r="R29" s="13"/>
@@ -2079,17 +2384,17 @@
       <c r="B30" s="24"/>
       <c r="C30" s="25"/>
       <c r="D30" s="26"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="48"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="50"/>
-      <c r="O30" s="47"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="47"/>
+      <c r="M30" s="47"/>
+      <c r="N30" s="48"/>
+      <c r="O30" s="45"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="13"/>
       <c r="R30" s="13"/>
@@ -2101,17 +2406,17 @@
       <c r="B31" s="24"/>
       <c r="C31" s="25"/>
       <c r="D31" s="26"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="48"/>
-      <c r="L31" s="49"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="50"/>
-      <c r="O31" s="47"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="46"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="48"/>
+      <c r="O31" s="45"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="13"/>
       <c r="R31" s="13"/>
@@ -2123,17 +2428,17 @@
       <c r="B32" s="24"/>
       <c r="C32" s="25"/>
       <c r="D32" s="26"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="41"/>
-      <c r="K32" s="48"/>
-      <c r="L32" s="49"/>
-      <c r="M32" s="49"/>
-      <c r="N32" s="50"/>
-      <c r="O32" s="47"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="46"/>
+      <c r="L32" s="47"/>
+      <c r="M32" s="47"/>
+      <c r="N32" s="48"/>
+      <c r="O32" s="45"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="13"/>
       <c r="R32" s="13"/>
@@ -2145,17 +2450,17 @@
       <c r="B33" s="24"/>
       <c r="C33" s="25"/>
       <c r="D33" s="26"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="48"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="49"/>
-      <c r="N33" s="50"/>
-      <c r="O33" s="47"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="39"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="47"/>
+      <c r="N33" s="48"/>
+      <c r="O33" s="45"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="13"/>
       <c r="R33" s="13"/>
@@ -2167,17 +2472,17 @@
       <c r="B34" s="24"/>
       <c r="C34" s="25"/>
       <c r="D34" s="26"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="49"/>
-      <c r="M34" s="49"/>
-      <c r="N34" s="50"/>
-      <c r="O34" s="47"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="46"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="48"/>
+      <c r="O34" s="45"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="13"/>
       <c r="R34" s="13"/>
@@ -2189,17 +2494,17 @@
       <c r="B35" s="24"/>
       <c r="C35" s="25"/>
       <c r="D35" s="26"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="39"/>
-      <c r="H35" s="40"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="38"/>
-      <c r="K35" s="48"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="49"/>
-      <c r="N35" s="50"/>
-      <c r="O35" s="47"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="36"/>
+      <c r="K35" s="46"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="48"/>
+      <c r="O35" s="45"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="13"/>
       <c r="R35" s="13"/>
@@ -2211,17 +2516,17 @@
       <c r="B36" s="24"/>
       <c r="C36" s="25"/>
       <c r="D36" s="26"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="39"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="48"/>
-      <c r="L36" s="49"/>
-      <c r="M36" s="49"/>
-      <c r="N36" s="50"/>
-      <c r="O36" s="47"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="39"/>
+      <c r="K36" s="46"/>
+      <c r="L36" s="47"/>
+      <c r="M36" s="47"/>
+      <c r="N36" s="48"/>
+      <c r="O36" s="45"/>
       <c r="P36" s="1"/>
       <c r="Q36" s="13"/>
       <c r="R36" s="13"/>
@@ -2233,17 +2538,17 @@
       <c r="B37" s="24"/>
       <c r="C37" s="25"/>
       <c r="D37" s="26"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="48"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="49"/>
-      <c r="N37" s="50"/>
-      <c r="O37" s="47"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="39"/>
+      <c r="K37" s="46"/>
+      <c r="L37" s="47"/>
+      <c r="M37" s="47"/>
+      <c r="N37" s="48"/>
+      <c r="O37" s="45"/>
       <c r="P37" s="1"/>
       <c r="Q37" s="13"/>
       <c r="R37" s="13"/>
@@ -2255,17 +2560,17 @@
       <c r="B38" s="24"/>
       <c r="C38" s="25"/>
       <c r="D38" s="26"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="48"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="49"/>
-      <c r="N38" s="50"/>
-      <c r="O38" s="47"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="39"/>
+      <c r="K38" s="46"/>
+      <c r="L38" s="47"/>
+      <c r="M38" s="47"/>
+      <c r="N38" s="48"/>
+      <c r="O38" s="45"/>
       <c r="P38" s="1"/>
       <c r="Q38" s="13"/>
       <c r="R38" s="13"/>
@@ -2277,17 +2582,17 @@
       <c r="B39" s="24"/>
       <c r="C39" s="25"/>
       <c r="D39" s="26"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="39"/>
-      <c r="H39" s="40"/>
-      <c r="I39" s="40"/>
-      <c r="J39" s="41"/>
-      <c r="K39" s="48"/>
-      <c r="L39" s="49"/>
-      <c r="M39" s="49"/>
-      <c r="N39" s="50"/>
-      <c r="O39" s="47"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="39"/>
+      <c r="K39" s="46"/>
+      <c r="L39" s="47"/>
+      <c r="M39" s="47"/>
+      <c r="N39" s="48"/>
+      <c r="O39" s="45"/>
       <c r="P39" s="1"/>
       <c r="Q39" s="13"/>
       <c r="R39" s="13"/>
@@ -2299,17 +2604,17 @@
       <c r="B40" s="24"/>
       <c r="C40" s="25"/>
       <c r="D40" s="26"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="33"/>
-      <c r="G40" s="39"/>
-      <c r="H40" s="40"/>
-      <c r="I40" s="40"/>
-      <c r="J40" s="41"/>
-      <c r="K40" s="48"/>
-      <c r="L40" s="49"/>
-      <c r="M40" s="49"/>
-      <c r="N40" s="50"/>
-      <c r="O40" s="47"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="46"/>
+      <c r="L40" s="47"/>
+      <c r="M40" s="47"/>
+      <c r="N40" s="48"/>
+      <c r="O40" s="45"/>
       <c r="P40" s="1"/>
       <c r="Q40" s="13"/>
       <c r="R40" s="13"/>
@@ -2321,17 +2626,17 @@
       <c r="B41" s="24"/>
       <c r="C41" s="25"/>
       <c r="D41" s="26"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="39"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="40"/>
-      <c r="J41" s="41"/>
-      <c r="K41" s="48"/>
-      <c r="L41" s="49"/>
-      <c r="M41" s="49"/>
-      <c r="N41" s="50"/>
-      <c r="O41" s="47"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="39"/>
+      <c r="K41" s="46"/>
+      <c r="L41" s="47"/>
+      <c r="M41" s="47"/>
+      <c r="N41" s="48"/>
+      <c r="O41" s="45"/>
       <c r="P41" s="1"/>
       <c r="Q41" s="13"/>
       <c r="R41" s="13"/>
@@ -2343,17 +2648,17 @@
       <c r="B42" s="24"/>
       <c r="C42" s="25"/>
       <c r="D42" s="26"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="40"/>
-      <c r="J42" s="41"/>
-      <c r="K42" s="48"/>
-      <c r="L42" s="49"/>
-      <c r="M42" s="49"/>
-      <c r="N42" s="50"/>
-      <c r="O42" s="47"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="46"/>
+      <c r="L42" s="47"/>
+      <c r="M42" s="47"/>
+      <c r="N42" s="48"/>
+      <c r="O42" s="45"/>
       <c r="P42" s="1"/>
       <c r="Q42" s="13"/>
       <c r="R42" s="13"/>
@@ -2365,17 +2670,17 @@
       <c r="B43" s="24"/>
       <c r="C43" s="25"/>
       <c r="D43" s="26"/>
-      <c r="E43" s="32"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="41"/>
-      <c r="K43" s="48"/>
-      <c r="L43" s="49"/>
-      <c r="M43" s="49"/>
-      <c r="N43" s="50"/>
-      <c r="O43" s="47"/>
+      <c r="E43" s="30"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="39"/>
+      <c r="K43" s="46"/>
+      <c r="L43" s="47"/>
+      <c r="M43" s="47"/>
+      <c r="N43" s="48"/>
+      <c r="O43" s="45"/>
       <c r="P43" s="1"/>
       <c r="Q43" s="13"/>
       <c r="R43" s="13"/>
@@ -2387,17 +2692,17 @@
       <c r="B44" s="24"/>
       <c r="C44" s="25"/>
       <c r="D44" s="26"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="41"/>
-      <c r="K44" s="48"/>
-      <c r="L44" s="49"/>
-      <c r="M44" s="49"/>
-      <c r="N44" s="50"/>
-      <c r="O44" s="47"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="39"/>
+      <c r="K44" s="46"/>
+      <c r="L44" s="47"/>
+      <c r="M44" s="47"/>
+      <c r="N44" s="48"/>
+      <c r="O44" s="45"/>
       <c r="P44" s="1"/>
       <c r="Q44" s="13"/>
       <c r="R44" s="13"/>
@@ -2408,18 +2713,18 @@
       <c r="A45" s="23"/>
       <c r="B45" s="24"/>
       <c r="C45" s="25"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="41"/>
-      <c r="K45" s="48"/>
-      <c r="L45" s="49"/>
-      <c r="M45" s="49"/>
-      <c r="N45" s="50"/>
-      <c r="O45" s="47"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="32"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="38"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="39"/>
+      <c r="K45" s="46"/>
+      <c r="L45" s="47"/>
+      <c r="M45" s="47"/>
+      <c r="N45" s="48"/>
+      <c r="O45" s="45"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="13"/>
       <c r="R45" s="13"/>
@@ -2430,18 +2735,18 @@
       <c r="A46" s="23"/>
       <c r="B46" s="24"/>
       <c r="C46" s="25"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="35"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="40"/>
-      <c r="I46" s="40"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="48"/>
-      <c r="L46" s="49"/>
-      <c r="M46" s="49"/>
-      <c r="N46" s="50"/>
-      <c r="O46" s="47"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="39"/>
+      <c r="K46" s="46"/>
+      <c r="L46" s="47"/>
+      <c r="M46" s="47"/>
+      <c r="N46" s="48"/>
+      <c r="O46" s="45"/>
       <c r="P46" s="1"/>
       <c r="Q46" s="13"/>
       <c r="R46" s="13"/>
@@ -2452,18 +2757,18 @@
       <c r="A47" s="23"/>
       <c r="B47" s="24"/>
       <c r="C47" s="25"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="35"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="40"/>
-      <c r="I47" s="40"/>
-      <c r="J47" s="41"/>
-      <c r="K47" s="48"/>
-      <c r="L47" s="49"/>
-      <c r="M47" s="49"/>
-      <c r="N47" s="50"/>
-      <c r="O47" s="47"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="33"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="39"/>
+      <c r="K47" s="46"/>
+      <c r="L47" s="47"/>
+      <c r="M47" s="47"/>
+      <c r="N47" s="48"/>
+      <c r="O47" s="45"/>
       <c r="P47" s="1"/>
       <c r="Q47" s="13"/>
       <c r="R47" s="13"/>
@@ -2474,18 +2779,18 @@
       <c r="A48" s="23"/>
       <c r="B48" s="24"/>
       <c r="C48" s="25"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="40"/>
-      <c r="J48" s="41"/>
-      <c r="K48" s="48"/>
-      <c r="L48" s="49"/>
-      <c r="M48" s="49"/>
-      <c r="N48" s="50"/>
-      <c r="O48" s="47"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="33"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="38"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="39"/>
+      <c r="K48" s="46"/>
+      <c r="L48" s="47"/>
+      <c r="M48" s="47"/>
+      <c r="N48" s="48"/>
+      <c r="O48" s="45"/>
       <c r="P48" s="1"/>
       <c r="Q48" s="13"/>
       <c r="R48" s="13"/>
@@ -2496,18 +2801,18 @@
       <c r="A49" s="23"/>
       <c r="B49" s="24"/>
       <c r="C49" s="25"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="39"/>
-      <c r="H49" s="40"/>
-      <c r="I49" s="40"/>
-      <c r="J49" s="41"/>
-      <c r="K49" s="48"/>
-      <c r="L49" s="49"/>
-      <c r="M49" s="49"/>
-      <c r="N49" s="50"/>
-      <c r="O49" s="47"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
+      <c r="J49" s="39"/>
+      <c r="K49" s="46"/>
+      <c r="L49" s="47"/>
+      <c r="M49" s="47"/>
+      <c r="N49" s="48"/>
+      <c r="O49" s="45"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="13"/>
       <c r="R49" s="13"/>
@@ -2518,18 +2823,18 @@
       <c r="A50" s="23"/>
       <c r="B50" s="24"/>
       <c r="C50" s="25"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="35"/>
-      <c r="G50" s="39"/>
-      <c r="H50" s="40"/>
-      <c r="I50" s="40"/>
-      <c r="J50" s="41"/>
-      <c r="K50" s="48"/>
-      <c r="L50" s="49"/>
-      <c r="M50" s="49"/>
-      <c r="N50" s="50"/>
-      <c r="O50" s="47"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="38"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="39"/>
+      <c r="K50" s="46"/>
+      <c r="L50" s="47"/>
+      <c r="M50" s="47"/>
+      <c r="N50" s="48"/>
+      <c r="O50" s="45"/>
       <c r="P50" s="1"/>
       <c r="Q50" s="13"/>
       <c r="R50" s="13"/>
@@ -2540,18 +2845,18 @@
       <c r="A51" s="23"/>
       <c r="B51" s="24"/>
       <c r="C51" s="25"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="35"/>
-      <c r="G51" s="39"/>
-      <c r="H51" s="40"/>
-      <c r="I51" s="40"/>
-      <c r="J51" s="41"/>
-      <c r="K51" s="48"/>
-      <c r="L51" s="49"/>
-      <c r="M51" s="49"/>
-      <c r="N51" s="50"/>
-      <c r="O51" s="47"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="33"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="38"/>
+      <c r="I51" s="38"/>
+      <c r="J51" s="39"/>
+      <c r="K51" s="46"/>
+      <c r="L51" s="47"/>
+      <c r="M51" s="47"/>
+      <c r="N51" s="48"/>
+      <c r="O51" s="45"/>
       <c r="P51" s="1"/>
       <c r="Q51" s="13"/>
       <c r="R51" s="13"/>
@@ -2562,18 +2867,18 @@
       <c r="A52" s="23"/>
       <c r="B52" s="24"/>
       <c r="C52" s="25"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="35"/>
-      <c r="G52" s="39"/>
-      <c r="H52" s="40"/>
-      <c r="I52" s="40"/>
-      <c r="J52" s="41"/>
-      <c r="K52" s="48"/>
-      <c r="L52" s="49"/>
-      <c r="M52" s="49"/>
-      <c r="N52" s="50"/>
-      <c r="O52" s="47"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
+      <c r="J52" s="39"/>
+      <c r="K52" s="46"/>
+      <c r="L52" s="47"/>
+      <c r="M52" s="47"/>
+      <c r="N52" s="48"/>
+      <c r="O52" s="45"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="13"/>
       <c r="R52" s="13"/>
@@ -2584,18 +2889,18 @@
       <c r="A53" s="23"/>
       <c r="B53" s="24"/>
       <c r="C53" s="25"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="35"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="40"/>
-      <c r="I53" s="40"/>
-      <c r="J53" s="41"/>
-      <c r="K53" s="48"/>
-      <c r="L53" s="49"/>
-      <c r="M53" s="49"/>
-      <c r="N53" s="50"/>
-      <c r="O53" s="47"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="32"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="39"/>
+      <c r="K53" s="46"/>
+      <c r="L53" s="47"/>
+      <c r="M53" s="47"/>
+      <c r="N53" s="48"/>
+      <c r="O53" s="45"/>
       <c r="P53" s="1"/>
       <c r="Q53" s="13"/>
       <c r="R53" s="13"/>
@@ -2606,18 +2911,18 @@
       <c r="A54" s="23"/>
       <c r="B54" s="24"/>
       <c r="C54" s="25"/>
-      <c r="D54" s="29"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="39"/>
-      <c r="H54" s="40"/>
-      <c r="I54" s="40"/>
-      <c r="J54" s="41"/>
-      <c r="K54" s="48"/>
-      <c r="L54" s="49"/>
-      <c r="M54" s="49"/>
-      <c r="N54" s="50"/>
-      <c r="O54" s="47"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="33"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="38"/>
+      <c r="J54" s="39"/>
+      <c r="K54" s="46"/>
+      <c r="L54" s="47"/>
+      <c r="M54" s="47"/>
+      <c r="N54" s="48"/>
+      <c r="O54" s="45"/>
       <c r="P54" s="1"/>
       <c r="Q54" s="13"/>
       <c r="R54" s="13"/>
@@ -2628,18 +2933,18 @@
       <c r="A55" s="23"/>
       <c r="B55" s="24"/>
       <c r="C55" s="25"/>
-      <c r="D55" s="29"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="39"/>
-      <c r="H55" s="40"/>
-      <c r="I55" s="40"/>
-      <c r="J55" s="41"/>
-      <c r="K55" s="48"/>
-      <c r="L55" s="49"/>
-      <c r="M55" s="49"/>
-      <c r="N55" s="50"/>
-      <c r="O55" s="47"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="38"/>
+      <c r="I55" s="38"/>
+      <c r="J55" s="39"/>
+      <c r="K55" s="46"/>
+      <c r="L55" s="47"/>
+      <c r="M55" s="47"/>
+      <c r="N55" s="48"/>
+      <c r="O55" s="45"/>
       <c r="P55" s="1"/>
       <c r="Q55" s="13"/>
       <c r="R55" s="13"/>
@@ -2650,18 +2955,18 @@
       <c r="A56" s="23"/>
       <c r="B56" s="24"/>
       <c r="C56" s="25"/>
-      <c r="D56" s="29"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="35"/>
-      <c r="G56" s="39"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="40"/>
-      <c r="J56" s="41"/>
-      <c r="K56" s="48"/>
-      <c r="L56" s="49"/>
-      <c r="M56" s="49"/>
-      <c r="N56" s="50"/>
-      <c r="O56" s="47"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="33"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+      <c r="J56" s="39"/>
+      <c r="K56" s="46"/>
+      <c r="L56" s="47"/>
+      <c r="M56" s="47"/>
+      <c r="N56" s="48"/>
+      <c r="O56" s="45"/>
       <c r="P56" s="1"/>
       <c r="Q56" s="13"/>
       <c r="R56" s="13"/>
@@ -2672,18 +2977,18 @@
       <c r="A57" s="23"/>
       <c r="B57" s="24"/>
       <c r="C57" s="25"/>
-      <c r="D57" s="29"/>
-      <c r="E57" s="34"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="39"/>
-      <c r="H57" s="40"/>
-      <c r="I57" s="40"/>
-      <c r="J57" s="41"/>
-      <c r="K57" s="48"/>
-      <c r="L57" s="49"/>
-      <c r="M57" s="49"/>
-      <c r="N57" s="50"/>
-      <c r="O57" s="47"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="33"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="38"/>
+      <c r="I57" s="38"/>
+      <c r="J57" s="39"/>
+      <c r="K57" s="46"/>
+      <c r="L57" s="47"/>
+      <c r="M57" s="47"/>
+      <c r="N57" s="48"/>
+      <c r="O57" s="45"/>
       <c r="P57" s="1"/>
       <c r="Q57" s="13"/>
       <c r="R57" s="13"/>
@@ -2694,18 +2999,18 @@
       <c r="A58" s="23"/>
       <c r="B58" s="24"/>
       <c r="C58" s="25"/>
-      <c r="D58" s="29"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="35"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="40"/>
-      <c r="I58" s="40"/>
-      <c r="J58" s="41"/>
-      <c r="K58" s="48"/>
-      <c r="L58" s="49"/>
-      <c r="M58" s="49"/>
-      <c r="N58" s="50"/>
-      <c r="O58" s="47"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="38"/>
+      <c r="I58" s="38"/>
+      <c r="J58" s="39"/>
+      <c r="K58" s="46"/>
+      <c r="L58" s="47"/>
+      <c r="M58" s="47"/>
+      <c r="N58" s="48"/>
+      <c r="O58" s="45"/>
       <c r="P58" s="1"/>
       <c r="Q58" s="13"/>
       <c r="R58" s="13"/>
@@ -2716,18 +3021,18 @@
       <c r="A59" s="23"/>
       <c r="B59" s="24"/>
       <c r="C59" s="25"/>
-      <c r="D59" s="29"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="35"/>
-      <c r="G59" s="39"/>
-      <c r="H59" s="40"/>
-      <c r="I59" s="40"/>
-      <c r="J59" s="41"/>
-      <c r="K59" s="48"/>
-      <c r="L59" s="49"/>
-      <c r="M59" s="49"/>
-      <c r="N59" s="50"/>
-      <c r="O59" s="47"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="32"/>
+      <c r="F59" s="33"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="38"/>
+      <c r="I59" s="38"/>
+      <c r="J59" s="39"/>
+      <c r="K59" s="46"/>
+      <c r="L59" s="47"/>
+      <c r="M59" s="47"/>
+      <c r="N59" s="48"/>
+      <c r="O59" s="45"/>
       <c r="P59" s="1"/>
       <c r="Q59" s="13"/>
       <c r="R59" s="13"/>
@@ -2738,18 +3043,18 @@
       <c r="A60" s="23"/>
       <c r="B60" s="24"/>
       <c r="C60" s="25"/>
-      <c r="D60" s="29"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="35"/>
-      <c r="G60" s="39"/>
-      <c r="H60" s="40"/>
-      <c r="I60" s="40"/>
-      <c r="J60" s="41"/>
-      <c r="K60" s="48"/>
-      <c r="L60" s="49"/>
-      <c r="M60" s="49"/>
-      <c r="N60" s="50"/>
-      <c r="O60" s="47"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="33"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="38"/>
+      <c r="I60" s="38"/>
+      <c r="J60" s="39"/>
+      <c r="K60" s="46"/>
+      <c r="L60" s="47"/>
+      <c r="M60" s="47"/>
+      <c r="N60" s="48"/>
+      <c r="O60" s="45"/>
       <c r="P60" s="1"/>
       <c r="Q60" s="13"/>
       <c r="R60" s="13"/>
@@ -2760,18 +3065,18 @@
       <c r="A61" s="23"/>
       <c r="B61" s="24"/>
       <c r="C61" s="25"/>
-      <c r="D61" s="29"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="35"/>
-      <c r="G61" s="39"/>
-      <c r="H61" s="40"/>
-      <c r="I61" s="40"/>
-      <c r="J61" s="41"/>
-      <c r="K61" s="48"/>
-      <c r="L61" s="49"/>
-      <c r="M61" s="49"/>
-      <c r="N61" s="50"/>
-      <c r="O61" s="47"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="33"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="38"/>
+      <c r="I61" s="38"/>
+      <c r="J61" s="39"/>
+      <c r="K61" s="46"/>
+      <c r="L61" s="47"/>
+      <c r="M61" s="47"/>
+      <c r="N61" s="48"/>
+      <c r="O61" s="45"/>
       <c r="P61" s="1"/>
       <c r="Q61" s="13"/>
       <c r="R61" s="13"/>
@@ -2782,18 +3087,18 @@
       <c r="A62" s="23"/>
       <c r="B62" s="24"/>
       <c r="C62" s="25"/>
-      <c r="D62" s="29"/>
-      <c r="E62" s="34"/>
-      <c r="F62" s="35"/>
-      <c r="G62" s="39"/>
-      <c r="H62" s="40"/>
-      <c r="I62" s="40"/>
-      <c r="J62" s="41"/>
-      <c r="K62" s="48"/>
-      <c r="L62" s="49"/>
-      <c r="M62" s="49"/>
-      <c r="N62" s="50"/>
-      <c r="O62" s="47"/>
+      <c r="D62" s="27"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="33"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="38"/>
+      <c r="I62" s="38"/>
+      <c r="J62" s="39"/>
+      <c r="K62" s="46"/>
+      <c r="L62" s="47"/>
+      <c r="M62" s="47"/>
+      <c r="N62" s="48"/>
+      <c r="O62" s="45"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="13"/>
       <c r="R62" s="13"/>
@@ -2804,18 +3109,18 @@
       <c r="A63" s="23"/>
       <c r="B63" s="24"/>
       <c r="C63" s="25"/>
-      <c r="D63" s="29"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="35"/>
-      <c r="G63" s="39"/>
-      <c r="H63" s="40"/>
-      <c r="I63" s="40"/>
-      <c r="J63" s="41"/>
-      <c r="K63" s="48"/>
-      <c r="L63" s="49"/>
-      <c r="M63" s="49"/>
-      <c r="N63" s="50"/>
-      <c r="O63" s="47"/>
+      <c r="D63" s="27"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="33"/>
+      <c r="G63" s="37"/>
+      <c r="H63" s="38"/>
+      <c r="I63" s="38"/>
+      <c r="J63" s="39"/>
+      <c r="K63" s="46"/>
+      <c r="L63" s="47"/>
+      <c r="M63" s="47"/>
+      <c r="N63" s="48"/>
+      <c r="O63" s="45"/>
       <c r="P63" s="1"/>
       <c r="Q63" s="13"/>
       <c r="R63" s="13"/>
@@ -2826,18 +3131,18 @@
       <c r="A64" s="23"/>
       <c r="B64" s="24"/>
       <c r="C64" s="25"/>
-      <c r="D64" s="29"/>
-      <c r="E64" s="34"/>
-      <c r="F64" s="35"/>
-      <c r="G64" s="39"/>
-      <c r="H64" s="40"/>
-      <c r="I64" s="40"/>
-      <c r="J64" s="41"/>
-      <c r="K64" s="48"/>
-      <c r="L64" s="49"/>
-      <c r="M64" s="49"/>
-      <c r="N64" s="50"/>
-      <c r="O64" s="47"/>
+      <c r="D64" s="27"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="33"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="39"/>
+      <c r="K64" s="46"/>
+      <c r="L64" s="47"/>
+      <c r="M64" s="47"/>
+      <c r="N64" s="48"/>
+      <c r="O64" s="45"/>
       <c r="P64" s="1"/>
       <c r="Q64" s="13"/>
       <c r="R64" s="13"/>
@@ -2848,18 +3153,18 @@
       <c r="A65" s="23"/>
       <c r="B65" s="24"/>
       <c r="C65" s="25"/>
-      <c r="D65" s="29"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="35"/>
-      <c r="G65" s="39"/>
-      <c r="H65" s="40"/>
-      <c r="I65" s="40"/>
-      <c r="J65" s="41"/>
-      <c r="K65" s="48"/>
-      <c r="L65" s="49"/>
-      <c r="M65" s="49"/>
-      <c r="N65" s="50"/>
-      <c r="O65" s="47"/>
+      <c r="D65" s="27"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="33"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="38"/>
+      <c r="I65" s="38"/>
+      <c r="J65" s="39"/>
+      <c r="K65" s="46"/>
+      <c r="L65" s="47"/>
+      <c r="M65" s="47"/>
+      <c r="N65" s="48"/>
+      <c r="O65" s="45"/>
       <c r="P65" s="1"/>
       <c r="Q65" s="13"/>
       <c r="R65" s="13"/>
@@ -2870,18 +3175,18 @@
       <c r="A66" s="23"/>
       <c r="B66" s="24"/>
       <c r="C66" s="25"/>
-      <c r="D66" s="29"/>
-      <c r="E66" s="34"/>
-      <c r="F66" s="35"/>
-      <c r="G66" s="39"/>
-      <c r="H66" s="40"/>
-      <c r="I66" s="40"/>
-      <c r="J66" s="41"/>
-      <c r="K66" s="48"/>
-      <c r="L66" s="49"/>
-      <c r="M66" s="49"/>
-      <c r="N66" s="50"/>
-      <c r="O66" s="47"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="32"/>
+      <c r="F66" s="33"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="38"/>
+      <c r="I66" s="38"/>
+      <c r="J66" s="39"/>
+      <c r="K66" s="46"/>
+      <c r="L66" s="47"/>
+      <c r="M66" s="47"/>
+      <c r="N66" s="48"/>
+      <c r="O66" s="45"/>
       <c r="P66" s="1"/>
       <c r="Q66" s="13"/>
       <c r="R66" s="13"/>
@@ -2892,18 +3197,18 @@
       <c r="A67" s="23"/>
       <c r="B67" s="24"/>
       <c r="C67" s="25"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="34"/>
-      <c r="F67" s="35"/>
-      <c r="G67" s="39"/>
-      <c r="H67" s="40"/>
-      <c r="I67" s="40"/>
-      <c r="J67" s="41"/>
-      <c r="K67" s="48"/>
-      <c r="L67" s="49"/>
-      <c r="M67" s="49"/>
-      <c r="N67" s="50"/>
-      <c r="O67" s="47"/>
+      <c r="D67" s="27"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="33"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="38"/>
+      <c r="I67" s="38"/>
+      <c r="J67" s="39"/>
+      <c r="K67" s="46"/>
+      <c r="L67" s="47"/>
+      <c r="M67" s="47"/>
+      <c r="N67" s="48"/>
+      <c r="O67" s="45"/>
       <c r="P67" s="1"/>
       <c r="Q67" s="13"/>
       <c r="R67" s="13"/>
@@ -2914,18 +3219,18 @@
       <c r="A68" s="23"/>
       <c r="B68" s="24"/>
       <c r="C68" s="25"/>
-      <c r="D68" s="29"/>
-      <c r="E68" s="34"/>
-      <c r="F68" s="35"/>
-      <c r="G68" s="39"/>
-      <c r="H68" s="40"/>
-      <c r="I68" s="40"/>
-      <c r="J68" s="41"/>
-      <c r="K68" s="48"/>
-      <c r="L68" s="49"/>
-      <c r="M68" s="49"/>
-      <c r="N68" s="50"/>
-      <c r="O68" s="47"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="33"/>
+      <c r="G68" s="37"/>
+      <c r="H68" s="38"/>
+      <c r="I68" s="38"/>
+      <c r="J68" s="39"/>
+      <c r="K68" s="46"/>
+      <c r="L68" s="47"/>
+      <c r="M68" s="47"/>
+      <c r="N68" s="48"/>
+      <c r="O68" s="45"/>
       <c r="P68" s="1"/>
       <c r="Q68" s="13"/>
       <c r="R68" s="13"/>
@@ -2936,18 +3241,18 @@
       <c r="A69" s="23"/>
       <c r="B69" s="24"/>
       <c r="C69" s="25"/>
-      <c r="D69" s="29"/>
-      <c r="E69" s="34"/>
-      <c r="F69" s="35"/>
-      <c r="G69" s="39"/>
-      <c r="H69" s="40"/>
-      <c r="I69" s="40"/>
-      <c r="J69" s="41"/>
-      <c r="K69" s="48"/>
-      <c r="L69" s="49"/>
-      <c r="M69" s="49"/>
-      <c r="N69" s="50"/>
-      <c r="O69" s="47"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="33"/>
+      <c r="G69" s="37"/>
+      <c r="H69" s="38"/>
+      <c r="I69" s="38"/>
+      <c r="J69" s="39"/>
+      <c r="K69" s="46"/>
+      <c r="L69" s="47"/>
+      <c r="M69" s="47"/>
+      <c r="N69" s="48"/>
+      <c r="O69" s="45"/>
       <c r="P69" s="1"/>
       <c r="Q69" s="13"/>
       <c r="R69" s="13"/>
@@ -2958,18 +3263,18 @@
       <c r="A70" s="23"/>
       <c r="B70" s="24"/>
       <c r="C70" s="25"/>
-      <c r="D70" s="29"/>
-      <c r="E70" s="34"/>
-      <c r="F70" s="35"/>
-      <c r="G70" s="39"/>
-      <c r="H70" s="40"/>
-      <c r="I70" s="40"/>
-      <c r="J70" s="41"/>
-      <c r="K70" s="48"/>
-      <c r="L70" s="49"/>
-      <c r="M70" s="49"/>
-      <c r="N70" s="50"/>
-      <c r="O70" s="47"/>
+      <c r="D70" s="27"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="33"/>
+      <c r="G70" s="37"/>
+      <c r="H70" s="38"/>
+      <c r="I70" s="38"/>
+      <c r="J70" s="39"/>
+      <c r="K70" s="46"/>
+      <c r="L70" s="47"/>
+      <c r="M70" s="47"/>
+      <c r="N70" s="48"/>
+      <c r="O70" s="45"/>
       <c r="P70" s="1"/>
       <c r="Q70" s="13"/>
       <c r="R70" s="13"/>
@@ -2980,18 +3285,18 @@
       <c r="A71" s="23"/>
       <c r="B71" s="24"/>
       <c r="C71" s="25"/>
-      <c r="D71" s="29"/>
-      <c r="E71" s="34"/>
-      <c r="F71" s="35"/>
-      <c r="G71" s="39"/>
-      <c r="H71" s="40"/>
-      <c r="I71" s="40"/>
-      <c r="J71" s="41"/>
-      <c r="K71" s="48"/>
-      <c r="L71" s="49"/>
-      <c r="M71" s="49"/>
-      <c r="N71" s="50"/>
-      <c r="O71" s="47"/>
+      <c r="D71" s="27"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="37"/>
+      <c r="H71" s="38"/>
+      <c r="I71" s="38"/>
+      <c r="J71" s="39"/>
+      <c r="K71" s="46"/>
+      <c r="L71" s="47"/>
+      <c r="M71" s="47"/>
+      <c r="N71" s="48"/>
+      <c r="O71" s="45"/>
       <c r="P71" s="1"/>
       <c r="Q71" s="13"/>
       <c r="R71" s="13"/>
@@ -3002,18 +3307,18 @@
       <c r="A72" s="23"/>
       <c r="B72" s="24"/>
       <c r="C72" s="25"/>
-      <c r="D72" s="29"/>
-      <c r="E72" s="34"/>
-      <c r="F72" s="35"/>
-      <c r="G72" s="39"/>
-      <c r="H72" s="40"/>
-      <c r="I72" s="40"/>
-      <c r="J72" s="41"/>
-      <c r="K72" s="48"/>
-      <c r="L72" s="49"/>
-      <c r="M72" s="49"/>
-      <c r="N72" s="50"/>
-      <c r="O72" s="47"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="33"/>
+      <c r="G72" s="37"/>
+      <c r="H72" s="38"/>
+      <c r="I72" s="38"/>
+      <c r="J72" s="39"/>
+      <c r="K72" s="46"/>
+      <c r="L72" s="47"/>
+      <c r="M72" s="47"/>
+      <c r="N72" s="48"/>
+      <c r="O72" s="45"/>
       <c r="P72" s="1"/>
       <c r="Q72" s="13"/>
       <c r="R72" s="13"/>
@@ -3024,18 +3329,18 @@
       <c r="A73" s="23"/>
       <c r="B73" s="24"/>
       <c r="C73" s="25"/>
-      <c r="D73" s="29"/>
-      <c r="E73" s="34"/>
-      <c r="F73" s="35"/>
-      <c r="G73" s="39"/>
-      <c r="H73" s="40"/>
-      <c r="I73" s="40"/>
-      <c r="J73" s="41"/>
-      <c r="K73" s="48"/>
-      <c r="L73" s="49"/>
-      <c r="M73" s="49"/>
-      <c r="N73" s="50"/>
-      <c r="O73" s="47"/>
+      <c r="D73" s="27"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="33"/>
+      <c r="G73" s="37"/>
+      <c r="H73" s="38"/>
+      <c r="I73" s="38"/>
+      <c r="J73" s="39"/>
+      <c r="K73" s="46"/>
+      <c r="L73" s="47"/>
+      <c r="M73" s="47"/>
+      <c r="N73" s="48"/>
+      <c r="O73" s="45"/>
       <c r="P73" s="1"/>
       <c r="Q73" s="13"/>
       <c r="R73" s="13"/>
@@ -3046,18 +3351,18 @@
       <c r="A74" s="23"/>
       <c r="B74" s="24"/>
       <c r="C74" s="25"/>
-      <c r="D74" s="29"/>
-      <c r="E74" s="34"/>
-      <c r="F74" s="35"/>
-      <c r="G74" s="39"/>
-      <c r="H74" s="40"/>
-      <c r="I74" s="40"/>
-      <c r="J74" s="41"/>
-      <c r="K74" s="48"/>
-      <c r="L74" s="49"/>
-      <c r="M74" s="49"/>
-      <c r="N74" s="50"/>
-      <c r="O74" s="47"/>
+      <c r="D74" s="27"/>
+      <c r="E74" s="32"/>
+      <c r="F74" s="33"/>
+      <c r="G74" s="37"/>
+      <c r="H74" s="38"/>
+      <c r="I74" s="38"/>
+      <c r="J74" s="39"/>
+      <c r="K74" s="46"/>
+      <c r="L74" s="47"/>
+      <c r="M74" s="47"/>
+      <c r="N74" s="48"/>
+      <c r="O74" s="45"/>
       <c r="P74" s="1"/>
       <c r="Q74" s="13"/>
       <c r="R74" s="13"/>
@@ -3068,18 +3373,18 @@
       <c r="A75" s="23"/>
       <c r="B75" s="24"/>
       <c r="C75" s="25"/>
-      <c r="D75" s="29"/>
-      <c r="E75" s="34"/>
-      <c r="F75" s="35"/>
-      <c r="G75" s="39"/>
-      <c r="H75" s="40"/>
-      <c r="I75" s="40"/>
-      <c r="J75" s="41"/>
-      <c r="K75" s="48"/>
-      <c r="L75" s="49"/>
-      <c r="M75" s="49"/>
-      <c r="N75" s="50"/>
-      <c r="O75" s="47"/>
+      <c r="D75" s="27"/>
+      <c r="E75" s="32"/>
+      <c r="F75" s="33"/>
+      <c r="G75" s="37"/>
+      <c r="H75" s="38"/>
+      <c r="I75" s="38"/>
+      <c r="J75" s="39"/>
+      <c r="K75" s="46"/>
+      <c r="L75" s="47"/>
+      <c r="M75" s="47"/>
+      <c r="N75" s="48"/>
+      <c r="O75" s="45"/>
       <c r="P75" s="1"/>
       <c r="Q75" s="13"/>
       <c r="R75" s="13"/>
@@ -3090,18 +3395,18 @@
       <c r="A76" s="23"/>
       <c r="B76" s="24"/>
       <c r="C76" s="25"/>
-      <c r="D76" s="29"/>
-      <c r="E76" s="34"/>
-      <c r="F76" s="35"/>
-      <c r="G76" s="39"/>
-      <c r="H76" s="40"/>
-      <c r="I76" s="40"/>
-      <c r="J76" s="41"/>
-      <c r="K76" s="48"/>
-      <c r="L76" s="49"/>
-      <c r="M76" s="49"/>
-      <c r="N76" s="50"/>
-      <c r="O76" s="47"/>
+      <c r="D76" s="27"/>
+      <c r="E76" s="32"/>
+      <c r="F76" s="33"/>
+      <c r="G76" s="37"/>
+      <c r="H76" s="38"/>
+      <c r="I76" s="38"/>
+      <c r="J76" s="39"/>
+      <c r="K76" s="46"/>
+      <c r="L76" s="47"/>
+      <c r="M76" s="47"/>
+      <c r="N76" s="48"/>
+      <c r="O76" s="45"/>
       <c r="P76" s="1"/>
       <c r="Q76" s="13"/>
       <c r="R76" s="13"/>
@@ -3112,18 +3417,18 @@
       <c r="A77" s="23"/>
       <c r="B77" s="24"/>
       <c r="C77" s="25"/>
-      <c r="D77" s="29"/>
-      <c r="E77" s="34"/>
-      <c r="F77" s="35"/>
-      <c r="G77" s="39"/>
-      <c r="H77" s="40"/>
-      <c r="I77" s="40"/>
-      <c r="J77" s="41"/>
-      <c r="K77" s="48"/>
-      <c r="L77" s="49"/>
-      <c r="M77" s="49"/>
-      <c r="N77" s="50"/>
-      <c r="O77" s="47"/>
+      <c r="D77" s="27"/>
+      <c r="E77" s="32"/>
+      <c r="F77" s="33"/>
+      <c r="G77" s="37"/>
+      <c r="H77" s="38"/>
+      <c r="I77" s="38"/>
+      <c r="J77" s="39"/>
+      <c r="K77" s="46"/>
+      <c r="L77" s="47"/>
+      <c r="M77" s="47"/>
+      <c r="N77" s="48"/>
+      <c r="O77" s="45"/>
       <c r="P77" s="1"/>
       <c r="Q77" s="13"/>
       <c r="R77" s="13"/>
@@ -3134,18 +3439,18 @@
       <c r="A78" s="23"/>
       <c r="B78" s="24"/>
       <c r="C78" s="25"/>
-      <c r="D78" s="29"/>
-      <c r="E78" s="34"/>
-      <c r="F78" s="35"/>
-      <c r="G78" s="39"/>
-      <c r="H78" s="40"/>
-      <c r="I78" s="40"/>
-      <c r="J78" s="41"/>
-      <c r="K78" s="48"/>
-      <c r="L78" s="49"/>
-      <c r="M78" s="49"/>
-      <c r="N78" s="50"/>
-      <c r="O78" s="47"/>
+      <c r="D78" s="27"/>
+      <c r="E78" s="32"/>
+      <c r="F78" s="33"/>
+      <c r="G78" s="37"/>
+      <c r="H78" s="38"/>
+      <c r="I78" s="38"/>
+      <c r="J78" s="39"/>
+      <c r="K78" s="46"/>
+      <c r="L78" s="47"/>
+      <c r="M78" s="47"/>
+      <c r="N78" s="48"/>
+      <c r="O78" s="45"/>
       <c r="P78" s="1"/>
       <c r="Q78" s="13"/>
       <c r="R78" s="13"/>
@@ -3156,18 +3461,18 @@
       <c r="A79" s="23"/>
       <c r="B79" s="24"/>
       <c r="C79" s="25"/>
-      <c r="D79" s="29"/>
-      <c r="E79" s="34"/>
-      <c r="F79" s="35"/>
-      <c r="G79" s="39"/>
-      <c r="H79" s="40"/>
-      <c r="I79" s="40"/>
-      <c r="J79" s="41"/>
-      <c r="K79" s="48"/>
-      <c r="L79" s="49"/>
-      <c r="M79" s="49"/>
-      <c r="N79" s="50"/>
-      <c r="O79" s="47"/>
+      <c r="D79" s="27"/>
+      <c r="E79" s="32"/>
+      <c r="F79" s="33"/>
+      <c r="G79" s="37"/>
+      <c r="H79" s="38"/>
+      <c r="I79" s="38"/>
+      <c r="J79" s="39"/>
+      <c r="K79" s="46"/>
+      <c r="L79" s="47"/>
+      <c r="M79" s="47"/>
+      <c r="N79" s="48"/>
+      <c r="O79" s="45"/>
       <c r="P79" s="1"/>
       <c r="Q79" s="13"/>
       <c r="R79" s="13"/>
@@ -3178,18 +3483,18 @@
       <c r="A80" s="23"/>
       <c r="B80" s="24"/>
       <c r="C80" s="25"/>
-      <c r="D80" s="29"/>
-      <c r="E80" s="34"/>
-      <c r="F80" s="35"/>
-      <c r="G80" s="39"/>
-      <c r="H80" s="40"/>
-      <c r="I80" s="40"/>
-      <c r="J80" s="41"/>
-      <c r="K80" s="48"/>
-      <c r="L80" s="49"/>
-      <c r="M80" s="49"/>
-      <c r="N80" s="50"/>
-      <c r="O80" s="47"/>
+      <c r="D80" s="27"/>
+      <c r="E80" s="32"/>
+      <c r="F80" s="33"/>
+      <c r="G80" s="37"/>
+      <c r="H80" s="38"/>
+      <c r="I80" s="38"/>
+      <c r="J80" s="39"/>
+      <c r="K80" s="46"/>
+      <c r="L80" s="47"/>
+      <c r="M80" s="47"/>
+      <c r="N80" s="48"/>
+      <c r="O80" s="45"/>
       <c r="P80" s="1"/>
       <c r="Q80" s="13"/>
       <c r="R80" s="13"/>
@@ -3200,18 +3505,18 @@
       <c r="A81" s="23"/>
       <c r="B81" s="24"/>
       <c r="C81" s="25"/>
-      <c r="D81" s="29"/>
-      <c r="E81" s="34"/>
-      <c r="F81" s="35"/>
-      <c r="G81" s="39"/>
-      <c r="H81" s="40"/>
-      <c r="I81" s="40"/>
-      <c r="J81" s="41"/>
-      <c r="K81" s="48"/>
-      <c r="L81" s="49"/>
-      <c r="M81" s="49"/>
-      <c r="N81" s="50"/>
-      <c r="O81" s="47"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="32"/>
+      <c r="F81" s="33"/>
+      <c r="G81" s="37"/>
+      <c r="H81" s="38"/>
+      <c r="I81" s="38"/>
+      <c r="J81" s="39"/>
+      <c r="K81" s="46"/>
+      <c r="L81" s="47"/>
+      <c r="M81" s="47"/>
+      <c r="N81" s="48"/>
+      <c r="O81" s="45"/>
       <c r="P81" s="1"/>
       <c r="Q81" s="13"/>
       <c r="R81" s="13"/>
@@ -3222,18 +3527,18 @@
       <c r="A82" s="23"/>
       <c r="B82" s="24"/>
       <c r="C82" s="25"/>
-      <c r="D82" s="29"/>
-      <c r="E82" s="34"/>
-      <c r="F82" s="35"/>
-      <c r="G82" s="39"/>
-      <c r="H82" s="40"/>
-      <c r="I82" s="40"/>
-      <c r="J82" s="41"/>
-      <c r="K82" s="48"/>
-      <c r="L82" s="49"/>
-      <c r="M82" s="49"/>
-      <c r="N82" s="50"/>
-      <c r="O82" s="47"/>
+      <c r="D82" s="27"/>
+      <c r="E82" s="32"/>
+      <c r="F82" s="33"/>
+      <c r="G82" s="37"/>
+      <c r="H82" s="38"/>
+      <c r="I82" s="38"/>
+      <c r="J82" s="39"/>
+      <c r="K82" s="46"/>
+      <c r="L82" s="47"/>
+      <c r="M82" s="47"/>
+      <c r="N82" s="48"/>
+      <c r="O82" s="45"/>
       <c r="P82" s="1"/>
       <c r="Q82" s="13"/>
       <c r="R82" s="13"/>
@@ -3244,18 +3549,18 @@
       <c r="A83" s="23"/>
       <c r="B83" s="24"/>
       <c r="C83" s="25"/>
-      <c r="D83" s="29"/>
-      <c r="E83" s="34"/>
-      <c r="F83" s="35"/>
-      <c r="G83" s="39"/>
-      <c r="H83" s="40"/>
-      <c r="I83" s="40"/>
-      <c r="J83" s="41"/>
-      <c r="K83" s="48"/>
-      <c r="L83" s="49"/>
-      <c r="M83" s="49"/>
-      <c r="N83" s="50"/>
-      <c r="O83" s="47"/>
+      <c r="D83" s="27"/>
+      <c r="E83" s="32"/>
+      <c r="F83" s="33"/>
+      <c r="G83" s="37"/>
+      <c r="H83" s="38"/>
+      <c r="I83" s="38"/>
+      <c r="J83" s="39"/>
+      <c r="K83" s="46"/>
+      <c r="L83" s="47"/>
+      <c r="M83" s="47"/>
+      <c r="N83" s="48"/>
+      <c r="O83" s="45"/>
       <c r="P83" s="1"/>
       <c r="Q83" s="13"/>
       <c r="R83" s="13"/>
@@ -3266,18 +3571,18 @@
       <c r="A84" s="23"/>
       <c r="B84" s="24"/>
       <c r="C84" s="25"/>
-      <c r="D84" s="29"/>
-      <c r="E84" s="34"/>
-      <c r="F84" s="35"/>
-      <c r="G84" s="39"/>
-      <c r="H84" s="40"/>
-      <c r="I84" s="40"/>
-      <c r="J84" s="41"/>
-      <c r="K84" s="48"/>
-      <c r="L84" s="49"/>
-      <c r="M84" s="49"/>
-      <c r="N84" s="50"/>
-      <c r="O84" s="47"/>
+      <c r="D84" s="27"/>
+      <c r="E84" s="32"/>
+      <c r="F84" s="33"/>
+      <c r="G84" s="37"/>
+      <c r="H84" s="38"/>
+      <c r="I84" s="38"/>
+      <c r="J84" s="39"/>
+      <c r="K84" s="46"/>
+      <c r="L84" s="47"/>
+      <c r="M84" s="47"/>
+      <c r="N84" s="48"/>
+      <c r="O84" s="45"/>
       <c r="P84" s="1"/>
       <c r="Q84" s="13"/>
       <c r="R84" s="13"/>
@@ -3288,18 +3593,18 @@
       <c r="A85" s="23"/>
       <c r="B85" s="24"/>
       <c r="C85" s="25"/>
-      <c r="D85" s="29"/>
-      <c r="E85" s="34"/>
-      <c r="F85" s="35"/>
-      <c r="G85" s="39"/>
-      <c r="H85" s="40"/>
-      <c r="I85" s="40"/>
-      <c r="J85" s="41"/>
-      <c r="K85" s="48"/>
-      <c r="L85" s="49"/>
-      <c r="M85" s="49"/>
-      <c r="N85" s="50"/>
-      <c r="O85" s="47"/>
+      <c r="D85" s="27"/>
+      <c r="E85" s="32"/>
+      <c r="F85" s="33"/>
+      <c r="G85" s="37"/>
+      <c r="H85" s="38"/>
+      <c r="I85" s="38"/>
+      <c r="J85" s="39"/>
+      <c r="K85" s="46"/>
+      <c r="L85" s="47"/>
+      <c r="M85" s="47"/>
+      <c r="N85" s="48"/>
+      <c r="O85" s="45"/>
       <c r="P85" s="1"/>
       <c r="Q85" s="13"/>
       <c r="R85" s="13"/>
@@ -3310,18 +3615,18 @@
       <c r="A86" s="23"/>
       <c r="B86" s="24"/>
       <c r="C86" s="25"/>
-      <c r="D86" s="29"/>
-      <c r="E86" s="34"/>
-      <c r="F86" s="35"/>
-      <c r="G86" s="39"/>
-      <c r="H86" s="40"/>
-      <c r="I86" s="40"/>
-      <c r="J86" s="41"/>
-      <c r="K86" s="48"/>
-      <c r="L86" s="49"/>
-      <c r="M86" s="49"/>
-      <c r="N86" s="50"/>
-      <c r="O86" s="47"/>
+      <c r="D86" s="27"/>
+      <c r="E86" s="32"/>
+      <c r="F86" s="33"/>
+      <c r="G86" s="37"/>
+      <c r="H86" s="38"/>
+      <c r="I86" s="38"/>
+      <c r="J86" s="39"/>
+      <c r="K86" s="46"/>
+      <c r="L86" s="47"/>
+      <c r="M86" s="47"/>
+      <c r="N86" s="48"/>
+      <c r="O86" s="45"/>
       <c r="P86" s="1"/>
       <c r="Q86" s="13"/>
       <c r="R86" s="13"/>
@@ -3332,18 +3637,18 @@
       <c r="A87" s="23"/>
       <c r="B87" s="24"/>
       <c r="C87" s="25"/>
-      <c r="D87" s="29"/>
-      <c r="E87" s="34"/>
-      <c r="F87" s="35"/>
-      <c r="G87" s="39"/>
-      <c r="H87" s="40"/>
-      <c r="I87" s="40"/>
-      <c r="J87" s="41"/>
-      <c r="K87" s="48"/>
-      <c r="L87" s="49"/>
-      <c r="M87" s="49"/>
-      <c r="N87" s="50"/>
-      <c r="O87" s="47"/>
+      <c r="D87" s="27"/>
+      <c r="E87" s="32"/>
+      <c r="F87" s="33"/>
+      <c r="G87" s="37"/>
+      <c r="H87" s="38"/>
+      <c r="I87" s="38"/>
+      <c r="J87" s="39"/>
+      <c r="K87" s="46"/>
+      <c r="L87" s="47"/>
+      <c r="M87" s="47"/>
+      <c r="N87" s="48"/>
+      <c r="O87" s="45"/>
       <c r="P87" s="1"/>
       <c r="Q87" s="13"/>
       <c r="R87" s="13"/>
@@ -3354,18 +3659,18 @@
       <c r="A88" s="23"/>
       <c r="B88" s="24"/>
       <c r="C88" s="25"/>
-      <c r="D88" s="29"/>
-      <c r="E88" s="34"/>
-      <c r="F88" s="35"/>
-      <c r="G88" s="39"/>
-      <c r="H88" s="40"/>
-      <c r="I88" s="40"/>
-      <c r="J88" s="41"/>
-      <c r="K88" s="48"/>
-      <c r="L88" s="49"/>
-      <c r="M88" s="49"/>
-      <c r="N88" s="50"/>
-      <c r="O88" s="47"/>
+      <c r="D88" s="27"/>
+      <c r="E88" s="32"/>
+      <c r="F88" s="33"/>
+      <c r="G88" s="37"/>
+      <c r="H88" s="38"/>
+      <c r="I88" s="38"/>
+      <c r="J88" s="39"/>
+      <c r="K88" s="46"/>
+      <c r="L88" s="47"/>
+      <c r="M88" s="47"/>
+      <c r="N88" s="48"/>
+      <c r="O88" s="45"/>
       <c r="P88" s="1"/>
       <c r="Q88" s="13"/>
       <c r="R88" s="13"/>
@@ -3376,18 +3681,18 @@
       <c r="A89" s="23"/>
       <c r="B89" s="24"/>
       <c r="C89" s="25"/>
-      <c r="D89" s="29"/>
-      <c r="E89" s="34"/>
-      <c r="F89" s="35"/>
-      <c r="G89" s="39"/>
-      <c r="H89" s="40"/>
-      <c r="I89" s="40"/>
-      <c r="J89" s="41"/>
-      <c r="K89" s="48"/>
-      <c r="L89" s="49"/>
-      <c r="M89" s="49"/>
-      <c r="N89" s="50"/>
-      <c r="O89" s="47"/>
+      <c r="D89" s="27"/>
+      <c r="E89" s="32"/>
+      <c r="F89" s="33"/>
+      <c r="G89" s="37"/>
+      <c r="H89" s="38"/>
+      <c r="I89" s="38"/>
+      <c r="J89" s="39"/>
+      <c r="K89" s="46"/>
+      <c r="L89" s="47"/>
+      <c r="M89" s="47"/>
+      <c r="N89" s="48"/>
+      <c r="O89" s="45"/>
       <c r="P89" s="1"/>
       <c r="Q89" s="13"/>
       <c r="R89" s="13"/>
@@ -3398,18 +3703,18 @@
       <c r="A90" s="23"/>
       <c r="B90" s="24"/>
       <c r="C90" s="25"/>
-      <c r="D90" s="29"/>
-      <c r="E90" s="34"/>
-      <c r="F90" s="35"/>
-      <c r="G90" s="39"/>
-      <c r="H90" s="40"/>
-      <c r="I90" s="40"/>
-      <c r="J90" s="41"/>
-      <c r="K90" s="48"/>
-      <c r="L90" s="49"/>
-      <c r="M90" s="49"/>
-      <c r="N90" s="50"/>
-      <c r="O90" s="47"/>
+      <c r="D90" s="27"/>
+      <c r="E90" s="32"/>
+      <c r="F90" s="33"/>
+      <c r="G90" s="37"/>
+      <c r="H90" s="38"/>
+      <c r="I90" s="38"/>
+      <c r="J90" s="39"/>
+      <c r="K90" s="46"/>
+      <c r="L90" s="47"/>
+      <c r="M90" s="47"/>
+      <c r="N90" s="48"/>
+      <c r="O90" s="45"/>
       <c r="P90" s="1"/>
       <c r="Q90" s="13"/>
       <c r="R90" s="13"/>

</xml_diff>